<commit_message>
adding proper sample data
</commit_message>
<xml_diff>
--- a/uploads/SCIJ_EXAMPLE_HEADERS.xlsx
+++ b/uploads/SCIJ_EXAMPLE_HEADERS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harid\Documents\Spring 2022\SCIJPartnerMatching\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harid\Documents\Spring 2022\SCIJPartnerMatching\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46420BA0-BB39-438A-BDBF-5F0956862D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6ED428-68EA-462A-8159-6B05910A5CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>header</t>
   </si>
@@ -64,19 +64,31 @@
   </si>
   <si>
     <t>Please describe your general availability next semester. [Friday]</t>
+  </si>
+  <si>
+    <t>Do you have a student you already would like to be paired with?</t>
+  </si>
+  <si>
+    <t>exclude_if "Yes"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,107 +394,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="A9:C9"/>
+      <selection activeCell="B10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>